<commit_message>
RTL Updates:    - prescaller - removed obsolete comments    - dco - updated registers and freq calculator excel    - dco - found 2 bugs wrong operation on clock gating and forgot to connect sfr inputs    - pwm&timer - fixed bug with wrong operation on clock gating cell    - various compilation errors fixed
Verification Updates:
   - added new test to the registers standard tests class
   - fixed compilation compilation error for cpu_reg_bank tb
   - implemented prescaller automated testbench and verified prescaller
   - implemented DCO automatic testbench and verified the DCO
   - renamed SFR directory to SFR_Tests
   - implemented dummy tests to the sfr testbench that will nedd to be updated later
</commit_message>
<xml_diff>
--- a/RTL/DCO/DCO Registers.xlsx
+++ b/RTL/DCO/DCO Registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\DCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A98319-A2D8-4FF1-8428-0BAEF1CFBA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD90DE62-A997-41B3-AE64-0B289B162694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="1695" windowWidth="14730" windowHeight="11385" xr2:uid="{C2F59BC8-B028-4C30-AFB2-8B1588A6E92D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2F59BC8-B028-4C30-AFB2-8B1588A6E92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>CLKSRC[1]</t>
   </si>
   <si>
-    <t>USESCLK</t>
-  </si>
-  <si>
     <t>HS</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>DCO_CNT</t>
+  </si>
+  <si>
+    <t>CLKSRC[2]</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3234D1-D8E4-42D2-A322-A69FD8618541}">
   <dimension ref="B2:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,28 +624,28 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -820,10 +820,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>12</v>
@@ -837,10 +837,10 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>14</v>
       </c>
@@ -964,7 +964,7 @@
     </row>
     <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1078,16 +1078,16 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1161,28 +1161,28 @@
     </row>
     <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1256,28 +1256,28 @@
     </row>
     <row r="47" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
RTL Updates:    - implemented wrapper for DCO 20 bit module    - updated sfr map with dco registers    - updated pipeline cpu top with dco and tmr instances, fixed typos
</commit_message>
<xml_diff>
--- a/RTL/DCO/DCO Registers.xlsx
+++ b/RTL/DCO/DCO Registers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosuv\Desktop\Disertatie\RISC-V_Microcontroller\RTL\DCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD90DE62-A997-41B3-AE64-0B289B162694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D7AAC8-F183-4B56-BBF6-868DCD20B779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2F59BC8-B028-4C30-AFB2-8B1588A6E92D}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3234D1-D8E4-42D2-A322-A69FD8618541}">
   <dimension ref="B2:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>